<commit_message>
handled edge case with flip cards should successfully detect the wrong side too
skipping queries on earlier cards is now done correctly. No longer wastes queries incorrectly

added fix to parse true for mistaken inputs

fixed default case for filename parsing
</commit_message>
<xml_diff>
--- a/Example Output.xlsx
+++ b/Example Output.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\campcapp\PycharmProjects\mtg_collection_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF112FBC-37D9-4011-8616-B566A1ACA710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F323F86-A3E3-4E6F-A499-5BCB5C510F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YURIKO CEDH" sheetId="1" r:id="rId1"/>
     <sheet name="SELVALA" sheetId="2" r:id="rId2"/>
-    <sheet name="Full Collection" sheetId="3" r:id="rId3"/>
+    <sheet name="Money Binder" sheetId="4" r:id="rId3"/>
+    <sheet name="Full Collection" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="364">
   <si>
     <t>Name</t>
   </si>
@@ -754,6 +755,366 @@
   </si>
   <si>
     <t>Shared?</t>
+  </si>
+  <si>
+    <t>Retribution of the Meek</t>
+  </si>
+  <si>
+    <t>Avacyn angel of hope</t>
+  </si>
+  <si>
+    <t>elesh norn grand cenobite</t>
+  </si>
+  <si>
+    <t>land tax</t>
+  </si>
+  <si>
+    <t>academy rector</t>
+  </si>
+  <si>
+    <t>replenish</t>
+  </si>
+  <si>
+    <t>serras sanctum</t>
+  </si>
+  <si>
+    <t>humility</t>
+  </si>
+  <si>
+    <t>annointed procession</t>
+  </si>
+  <si>
+    <t>smothering tithe</t>
+  </si>
+  <si>
+    <t>test of endurance</t>
+  </si>
+  <si>
+    <t>opalescence</t>
+  </si>
+  <si>
+    <t>reconnaissance</t>
+  </si>
+  <si>
+    <t>Heliod god of the sun</t>
+  </si>
+  <si>
+    <t>Divine Visitation</t>
+  </si>
+  <si>
+    <t>palace jailer</t>
+  </si>
+  <si>
+    <t>cathar's crusade</t>
+  </si>
+  <si>
+    <t>sram, senior edificer</t>
+  </si>
+  <si>
+    <t>palinchron</t>
+  </si>
+  <si>
+    <t>mind over matter</t>
+  </si>
+  <si>
+    <t>dream halls</t>
+  </si>
+  <si>
+    <t>rhystic study</t>
+  </si>
+  <si>
+    <t>treachery</t>
+  </si>
+  <si>
+    <t>sun quan, lord of wu</t>
+  </si>
+  <si>
+    <t>brainstorm</t>
+  </si>
+  <si>
+    <t>ss1</t>
+  </si>
+  <si>
+    <t>jin-gitaxias, core augur</t>
+  </si>
+  <si>
+    <t>true-name nemesis</t>
+  </si>
+  <si>
+    <t>Faerie Artisans</t>
+  </si>
+  <si>
+    <t>Omniscience</t>
+  </si>
+  <si>
+    <t>Teferi, Mage of Zhalfir</t>
+  </si>
+  <si>
+    <t>Myojin of night's reach</t>
+  </si>
+  <si>
+    <t>herald of leshrac</t>
+  </si>
+  <si>
+    <t>diabolic intent</t>
+  </si>
+  <si>
+    <t>urborg, tomb of yawgmoth</t>
+  </si>
+  <si>
+    <t>cabal coffers</t>
+  </si>
+  <si>
+    <t>rune-scarred demon</t>
+  </si>
+  <si>
+    <t>entomb</t>
+  </si>
+  <si>
+    <t>g11</t>
+  </si>
+  <si>
+    <t>haunted crossroads</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>necropotence</t>
+  </si>
+  <si>
+    <t>necromancy</t>
+  </si>
+  <si>
+    <t>razaketh, the foul blooded</t>
+  </si>
+  <si>
+    <t>bloodghast</t>
+  </si>
+  <si>
+    <t>liliana, heretical healer</t>
+  </si>
+  <si>
+    <t>nirkana revenant</t>
+  </si>
+  <si>
+    <t>archfiend of despair</t>
+  </si>
+  <si>
+    <t>dictate of erebos</t>
+  </si>
+  <si>
+    <t>exsanguinate</t>
+  </si>
+  <si>
+    <t>vilis, broker of blood</t>
+  </si>
+  <si>
+    <t>animate dead</t>
+  </si>
+  <si>
+    <t>liliana vess</t>
+  </si>
+  <si>
+    <t>bloodline keeper</t>
+  </si>
+  <si>
+    <t>pyroblast</t>
+  </si>
+  <si>
+    <t>hellkite tyrant</t>
+  </si>
+  <si>
+    <t>insurrection</t>
+  </si>
+  <si>
+    <t>world gorger dragon</t>
+  </si>
+  <si>
+    <t>urabrask, the hidden</t>
+  </si>
+  <si>
+    <t>bonus round</t>
+  </si>
+  <si>
+    <t>vigor</t>
+  </si>
+  <si>
+    <t>seasons past</t>
+  </si>
+  <si>
+    <t>ramunap excavator</t>
+  </si>
+  <si>
+    <t>triumph of the hordes</t>
+  </si>
+  <si>
+    <t>exploration</t>
+  </si>
+  <si>
+    <t>heroic intervention</t>
+  </si>
+  <si>
+    <t>Kindred Summons</t>
+  </si>
+  <si>
+    <t>Eternal witness</t>
+  </si>
+  <si>
+    <t>avenger of zendikar</t>
+  </si>
+  <si>
+    <t>nylea, god of the hunt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bramble sovereign </t>
+  </si>
+  <si>
+    <t>doubling season</t>
+  </si>
+  <si>
+    <t>yavimaya hollow</t>
+  </si>
+  <si>
+    <t>rofellos, llanowar emissary</t>
+  </si>
+  <si>
+    <t>aluren</t>
+  </si>
+  <si>
+    <t>burgeoning</t>
+  </si>
+  <si>
+    <t>arachnogenesis</t>
+  </si>
+  <si>
+    <t>vorinclex, voice of hunger</t>
+  </si>
+  <si>
+    <t>eladamri, lord of leaves</t>
+  </si>
+  <si>
+    <t>lotus cobra</t>
+  </si>
+  <si>
+    <t>city of solitude</t>
+  </si>
+  <si>
+    <t>seedborn muse</t>
+  </si>
+  <si>
+    <t>memory jar</t>
+  </si>
+  <si>
+    <t>windswept heath</t>
+  </si>
+  <si>
+    <t>bountiful promenade</t>
+  </si>
+  <si>
+    <t>hallowed fountain</t>
+  </si>
+  <si>
+    <t>high market</t>
+  </si>
+  <si>
+    <t>wooded foothills</t>
+  </si>
+  <si>
+    <t>spire garden</t>
+  </si>
+  <si>
+    <t>prime speaker zegana</t>
+  </si>
+  <si>
+    <t>blood crypt</t>
+  </si>
+  <si>
+    <t>godless shrine</t>
+  </si>
+  <si>
+    <t>overgrown tomb</t>
+  </si>
+  <si>
+    <t>static orb</t>
+  </si>
+  <si>
+    <t>command beacon</t>
+  </si>
+  <si>
+    <t>akroma's memorial</t>
+  </si>
+  <si>
+    <t>sword of feast and famine</t>
+  </si>
+  <si>
+    <t>metalworker</t>
+  </si>
+  <si>
+    <t>crucible of worlds</t>
+  </si>
+  <si>
+    <t>vedalken orrery</t>
+  </si>
+  <si>
+    <t>master of cruelties</t>
+  </si>
+  <si>
+    <t>aura shards</t>
+  </si>
+  <si>
+    <t>luxury suite</t>
+  </si>
+  <si>
+    <t>rhys, the redeemed</t>
+  </si>
+  <si>
+    <t>ulamog, the infinite gyre</t>
+  </si>
+  <si>
+    <t>ezuri, claw of progress</t>
+  </si>
+  <si>
+    <t>herald's horn</t>
+  </si>
+  <si>
+    <t>winding canyons</t>
+  </si>
+  <si>
+    <t>strip mine</t>
+  </si>
+  <si>
+    <t>kruphix, god of horizons</t>
+  </si>
+  <si>
+    <t>miraris wake</t>
+  </si>
+  <si>
+    <t>sterling grove</t>
+  </si>
+  <si>
+    <t>rashmi, eternities crafter</t>
+  </si>
+  <si>
+    <t>squandered resources</t>
+  </si>
+  <si>
+    <t>skullclamp</t>
+  </si>
+  <si>
+    <t>iroas, god of victory</t>
+  </si>
+  <si>
+    <t>panharmonicon</t>
+  </si>
+  <si>
+    <t>ashnod's altar</t>
+  </si>
+  <si>
+    <t>helm of the host</t>
+  </si>
+  <si>
+    <t>coat of arms</t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3644,6 +4005,683 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4DBC34-3D05-4272-92B9-4FC47F302459}">
+  <dimension ref="A1:F118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26" t="s">
+        <v>269</v>
+      </c>
+      <c r="C26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" t="s">
+        <v>282</v>
+      </c>
+      <c r="C38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>283</v>
+      </c>
+      <c r="C39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>293</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>325</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>327</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>331</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>334</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>335</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>341</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>344</v>
+      </c>
+      <c r="C99" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>346</v>
+      </c>
+      <c r="C101" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>356</v>
+      </c>
+      <c r="C111" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>358</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>360</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>361</v>
+      </c>
+      <c r="D116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>363</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>

</xml_diff>